<commit_message>
Update example Excel data files.
</commit_message>
<xml_diff>
--- a/clean_data.xlsx
+++ b/clean_data.xlsx
@@ -461,135 +461,135 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cooling-Tower</t>
+          <t>Turbine-A</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>176.08</v>
+        <v>293.67</v>
       </c>
       <c r="C2" t="n">
-        <v>133.93</v>
+        <v>156.4</v>
       </c>
       <c r="D2" t="n">
-        <v>324.45</v>
+        <v>303.3</v>
       </c>
       <c r="E2" t="n">
-        <v>2772.21</v>
+        <v>2403.29</v>
       </c>
       <c r="F2" t="n">
-        <v>19.84</v>
+        <v>25.18</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>86.8%</t>
+          <t>86.2%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Turbine-A</t>
+          <t>Boiler-2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>479.02</v>
+        <v>187.05</v>
       </c>
       <c r="C3" t="n">
-        <v>95.7</v>
+        <v>147.76</v>
       </c>
       <c r="D3" t="n">
-        <v>406.39</v>
+        <v>307.69</v>
       </c>
       <c r="E3" t="n">
-        <v>4692.22</v>
+        <v>3835.14</v>
       </c>
       <c r="F3" t="n">
-        <v>44</v>
+        <v>42.2</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>88.2%</t>
+          <t>94.6%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Boiler-1</t>
+          <t>Turbine-A</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>240.39</v>
+        <v>459.68</v>
       </c>
       <c r="C4" t="n">
-        <v>191.4</v>
+        <v>50.75</v>
       </c>
       <c r="D4" t="n">
-        <v>370.56</v>
+        <v>426.35</v>
       </c>
       <c r="E4" t="n">
-        <v>4630.96</v>
+        <v>1795.1</v>
       </c>
       <c r="F4" t="n">
-        <v>30.52</v>
+        <v>29.14</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>89.1%</t>
+          <t>88.7%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cooling-Tower</t>
+          <t>Turbine-A</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>225.48</v>
+        <v>447.51</v>
       </c>
       <c r="C5" t="n">
-        <v>209.62</v>
+        <v>84.31999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>348.95</v>
+        <v>449.87</v>
       </c>
       <c r="E5" t="n">
-        <v>3092.36</v>
+        <v>2114.78</v>
       </c>
       <c r="F5" t="n">
-        <v>44.51</v>
+        <v>36.42</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>78.9%</t>
+          <t>91.7%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Boiler-1</t>
+          <t>Cooling-Tower</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>231.8</v>
+        <v>336.46</v>
       </c>
       <c r="C6" t="n">
-        <v>125.66</v>
+        <v>149.1</v>
       </c>
       <c r="D6" t="n">
-        <v>333.39</v>
+        <v>347.61</v>
       </c>
       <c r="E6" t="n">
-        <v>1338.71</v>
+        <v>1985.8</v>
       </c>
       <c r="F6" t="n">
-        <v>25.23</v>
+        <v>26.09</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>89.7%</t>
+          <t>89.5%</t>
         </is>
       </c>
     </row>

</xml_diff>